<commit_message>
24/01/23 -> Scripting DPLKINV010-001 and DPLKINV011-001 25/01/23 -> Scripting DPLKINV001-001, DPLKINV002-001, DPLKINV003-001 26/01/23 -> Scripting DPLKINV004-001, DPLKINV005-001, DPLKINV006-001, DPLKINV007-001 AND DPLKKPS131-001, DPLKKPS132-001, DPLKKPS133-001, DPLKKPS134-001 27/01/23 -> Scripting DPLKINV008-001, DPLKINV009-001, DPLKINV010-001, DPLKINV011-001, DPLKINV012-001, DPLKINV013-001, DPLKINV014-001
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV006-001 - Investasi - Fixed Income - Tambah Dealing Ticket Fixed Income.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV006-001 - Investasi - Fixed Income - Tambah Dealing Ticket Fixed Income.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19017F32-A5FE-4B59-8626-BC18507C5441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EFDA3E-0943-45A9-B568-F62387C267C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -612,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>